<commit_message>
Add qr code generation to send sms for birthdays
</commit_message>
<xml_diff>
--- a/BirthDates.xlsx
+++ b/BirthDates.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ENDI\Documents\UiPath\Birthday Reminder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E031CA-F725-425C-8878-258E1DEA492C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7EAF24B-FB82-474E-BAE8-15B86C5E66E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="4155" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5070" yWindow="3465" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Birthdate</t>
   </si>
@@ -46,6 +46,24 @@
   </si>
   <si>
     <t>Memos</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>+903688392681</t>
+  </si>
+  <si>
+    <t>+903421381838</t>
+  </si>
+  <si>
+    <t>+905459416411</t>
+  </si>
+  <si>
+    <t>+904888931152</t>
+  </si>
+  <si>
+    <t>+903623489304</t>
   </si>
 </sst>
 </file>
@@ -81,9 +99,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -364,66 +383,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1">
         <v>34700</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1">
         <v>38880</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>45285</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1">
-        <v>27733</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>27734</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="1">
-        <v>28829</v>
+        <v>28830</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="C2:C6" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>